<commit_message>
Various changes to Filter Design
</commit_message>
<xml_diff>
--- a/electronics/receiver/FilterDesign/145MHz BPF DesignV3.xlsx
+++ b/electronics/receiver/FilterDesign/145MHz BPF DesignV3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\GitHub\pi-transceiver\NewPIT\pi-transceiver\electronics\receiver\FilterDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C995C6-97F5-41F1-AEF5-159BEBE2ABCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB051473-0EDE-4FCF-8A6C-90A5EEE70BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{058A02D5-4906-48D4-ADA1-9B0F3222F64A}"/>
   </bookViews>
@@ -9717,7 +9717,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9763,7 +9763,7 @@
         <v>0.66666666666666652</v>
       </c>
       <c r="F20">
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
       <c r="H20">
         <v>4.9000000000000004</v>
@@ -9778,7 +9778,7 @@
         <v>0.41666666666666663</v>
       </c>
       <c r="F21">
-        <v>0.33496100000000001</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="H21">
         <v>0.33300000000000002</v>
@@ -9793,7 +9793,7 @@
         <v>0.66666666666666652</v>
       </c>
       <c r="F22">
-        <v>0.2</v>
+        <v>0.34</v>
       </c>
       <c r="H22">
         <v>4.9000000000000004</v>
@@ -9811,7 +9811,7 @@
       </c>
       <c r="F24">
         <f>(F20*F21+F20*F22+F21*F22)/F21</f>
-        <v>0.51941688733912306</v>
+        <v>0.50119402985074635</v>
       </c>
       <c r="H24">
         <f>(H20*H21+H20*H22+H21*H22)/H21</f>
@@ -9827,7 +9827,7 @@
       </c>
       <c r="F25">
         <f>(F20*F21+F20*F22+F21*F22)/F22</f>
-        <v>0.86992199999999997</v>
+        <v>0.49382352941176472</v>
       </c>
       <c r="H25">
         <f>(H20*H21+H20*H22+H21*H22)/H22</f>
@@ -9843,7 +9843,7 @@
       </c>
       <c r="F26">
         <f>(F20*F21+F20*F22+F21*F22)/F20</f>
-        <v>0.86992199999999997</v>
+        <v>2.0987500000000003</v>
       </c>
       <c r="H26">
         <f>(H20*H21+H20*H22+H21*H22)/H20</f>
@@ -43901,7 +43901,7 @@
   <dimension ref="A1:AG37"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>